<commit_message>
changer screenshot et guide
</commit_message>
<xml_diff>
--- a/screenshot Site/Liste screenshot.xlsx
+++ b/screenshot Site/Liste screenshot.xlsx
@@ -184,10 +184,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,7 +505,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,16 +517,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="6" t="s">
         <v>24</v>
       </c>
     </row>
@@ -534,10 +534,10 @@
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>14</v>
       </c>
     </row>
@@ -545,10 +545,10 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -556,10 +556,10 @@
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -567,10 +567,10 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -579,7 +579,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -588,7 +588,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>